<commit_message>
I conducted a qualitative analysis. I created a table of incorrect questions. I compiled the questions into a table and created a diagram for it.
</commit_message>
<xml_diff>
--- a/kvalitativ/kerdesek_valaszok.xlsx
+++ b/kvalitativ/kerdesek_valaszok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krisztina_PC\flask-chatbot\kvalitativ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E5DD7C1-C20E-4F2E-86AD-F748ED9F79C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACBF06D-C1A1-4F10-A10C-FD604A1A5477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DEF7892C-22C1-4F84-9512-E9C698CC4EB2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Kérdés</t>
   </si>
@@ -147,15 +147,6 @@
   </si>
   <si>
     <t>200 lej/fő</t>
-  </si>
-  <si>
-    <t>Mi a fő célja a többciklusú képzés rendszernak?</t>
-  </si>
-  <si>
-    <t>A Bologna-folyamat célja az európai felsőoktatás ésszerű harmonizációja.</t>
-  </si>
-  <si>
-    <t>Fő célja, hogy lehetővé tegye a munkaerőpiacon való elhelyezkedést biztosító diploma megszerzését, ezért az alapképzés során a gyakorlati képzés kap nagyobb hangsúlyt.</t>
   </si>
   <si>
     <t>Kik a matinfo tanársegédei?</t>
@@ -260,9 +251,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -271,8 +262,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2EE712-B94B-4470-B617-89140A2869B9}">
-  <dimension ref="B6:F22"/>
+  <dimension ref="B6:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,8 +802,8 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
+    <row r="17" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -822,11 +816,11 @@
         <v>36</v>
       </c>
       <c r="F17" s="4">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="3">
+      <c r="B18" s="5">
         <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -839,11 +833,11 @@
         <v>39</v>
       </c>
       <c r="F18" s="4">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="3">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -852,61 +846,44 @@
       <c r="D19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="4">
+        <v>15</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="4">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="3">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4">
+        <v>50</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="4">
-        <v>15</v>
-      </c>
-      <c r="F20" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B21" s="3">
-        <v>15</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="E21" s="4">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="F21" s="4">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="3">
-        <v>16</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="4">
-        <v>6</v>
-      </c>
-      <c r="F22" s="4">
         <v>0.48</v>
       </c>
     </row>

</xml_diff>